<commit_message>
Add passif validation pipeline + improved logging
</commit_message>
<xml_diff>
--- a/COMPAGNIE_MEDITERRANEENNE_D_ASSURANCES_ET_DE_REASSURANCES_-_COMAR_-_2024_actif_Etats_financiers_au_31_12.xlsx
+++ b/COMPAGNIE_MEDITERRANEENNE_D_ASSURANCES_ET_DE_REASSURANCES_-_COMAR_-_2024_actif_Etats_financiers_au_31_12.xlsx
@@ -473,11 +473,6 @@
           <t>NET_N1 2023</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>EXTRA</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">

</xml_diff>